<commit_message>
Update the column name for all campus
</commit_message>
<xml_diff>
--- a/Mapping/unimelb_burnley_url.xlsx
+++ b/Mapping/unimelb_burnley_url.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
-    <t>Building name</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>url</t>
+    <t>building_name</t>
+  </si>
+  <si>
+    <t>building_no</t>
+  </si>
+  <si>
+    <t>website:map</t>
   </si>
   <si>
     <t>BURNLEY QUADRANGLE BUILDING 6</t>
@@ -103,43 +103,43 @@
     <t>917</t>
   </si>
   <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 898 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 901 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 899 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 902 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 903 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 905 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 906 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 907 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 908 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 911 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 914 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 916 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi= 917 </t>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=898</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=901</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=899</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=902</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=903</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=905</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=906</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=907</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=908</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=911</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=914</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=916</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=218&amp;sharepoitype=identifier&amp;sharepoi=917</t>
   </si>
 </sst>
 </file>

</xml_diff>